<commit_message>
update ltpp and ngcs
</commit_message>
<xml_diff>
--- a/special_sections/LTTP_sections/excel_files/ltpp_sections_info.xlsx
+++ b/special_sections/LTTP_sections/excel_files/ltpp_sections_info.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://texastechuniversity-my.sharepoint.com/personal/samuel_alalade_ttu_edu/Documents/Research/PhD/0-7147/Tasks/Task 9/Shared FIles/rpdb/sections_info/special_sections/ltpp_sections/excel_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://texastechuniversity-my.sharepoint.com/personal/samuel_alalade_ttu_edu/Documents/Research/PhD/0-7147/Tasks/Task 9/Shared FIles/rpdb/sections_info/special_sections/LTTP_sections/excel_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="42" documentId="11_7E9101E8F613C8A648227C7B1B36CCDC7552D82B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{691D365C-A692-4AF1-88EA-99E4A324B9B0}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="11_7E9101E8F613C8A648227C7B1B36CCDC7552D82B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A33EE702-8F05-4014-8599-C711651492D5}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="255" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="107">
   <si>
     <t>Section Data Type</t>
   </si>
@@ -189,6 +189,171 @@
   </si>
   <si>
     <t>Loop 289</t>
+  </si>
+  <si>
+    <t>48-3779-US54-LTPP</t>
+  </si>
+  <si>
+    <t>US 54</t>
+  </si>
+  <si>
+    <t>El Paso</t>
+  </si>
+  <si>
+    <t>31.790822, -106.440705</t>
+  </si>
+  <si>
+    <t>48-5278-BI20E-LTPP</t>
+  </si>
+  <si>
+    <t>BI 20E</t>
+  </si>
+  <si>
+    <t>Odessa</t>
+  </si>
+  <si>
+    <t>Ector</t>
+  </si>
+  <si>
+    <t>31.925035, -102.213078</t>
+  </si>
+  <si>
+    <t>48-1096-US90-LTPP</t>
+  </si>
+  <si>
+    <t>US 90</t>
+  </si>
+  <si>
+    <t>San Antonio</t>
+  </si>
+  <si>
+    <t>Bexar</t>
+  </si>
+  <si>
+    <t>29.35514067,-98.83470903</t>
+  </si>
+  <si>
+    <t>29.69240860,-97.23887494</t>
+  </si>
+  <si>
+    <t>48-5024-SH71-LTPP</t>
+  </si>
+  <si>
+    <t>SH 71</t>
+  </si>
+  <si>
+    <t>Colorado</t>
+  </si>
+  <si>
+    <t>29.73128995,-96.58131749</t>
+  </si>
+  <si>
+    <t>48-3010-SH146-LTPP</t>
+  </si>
+  <si>
+    <t>SH 146</t>
+  </si>
+  <si>
+    <t>Houston</t>
+  </si>
+  <si>
+    <t>Harris</t>
+  </si>
+  <si>
+    <t>29.79191853,-94.90662801</t>
+  </si>
+  <si>
+    <t>48-0802-FM2223-LTPP</t>
+  </si>
+  <si>
+    <t>FM 2223</t>
+  </si>
+  <si>
+    <t>Bryan</t>
+  </si>
+  <si>
+    <t>Brazos</t>
+  </si>
+  <si>
+    <t>30.78784069,-96.41133312</t>
+  </si>
+  <si>
+    <t>48-A808-SH195-LTPP</t>
+  </si>
+  <si>
+    <t>SH 195</t>
+  </si>
+  <si>
+    <t>Waco</t>
+  </si>
+  <si>
+    <t>Bell</t>
+  </si>
+  <si>
+    <t>30.98926033,-97.76215001</t>
+  </si>
+  <si>
+    <t>48-5284-SH121-LTPP</t>
+  </si>
+  <si>
+    <t>SH 121</t>
+  </si>
+  <si>
+    <t>Fort Worth</t>
+  </si>
+  <si>
+    <t>Tarrant</t>
+  </si>
+  <si>
+    <t>32.90914988,-97.09772845</t>
+  </si>
+  <si>
+    <t>48-5283-SH121-LTPP</t>
+  </si>
+  <si>
+    <t>32.86419812,-97.10191135</t>
+  </si>
+  <si>
+    <t>48-5317-US287-LTPP</t>
+  </si>
+  <si>
+    <t>US 287</t>
+  </si>
+  <si>
+    <t>32.59556183,-97.14614634</t>
+  </si>
+  <si>
+    <t>48-5301-IH820-LTPP</t>
+  </si>
+  <si>
+    <t>IH 820</t>
+  </si>
+  <si>
+    <t>32.71449651,-97.47855896</t>
+  </si>
+  <si>
+    <t>48-5310-US380-LTPP</t>
+  </si>
+  <si>
+    <t>US 380</t>
+  </si>
+  <si>
+    <t>Wise</t>
+  </si>
+  <si>
+    <t>33.23338830,-97.60971429</t>
+  </si>
+  <si>
+    <t>48-5328-US287-LTPP</t>
+  </si>
+  <si>
+    <t>Wichita Falls</t>
+  </si>
+  <si>
+    <t>Montague</t>
+  </si>
+  <si>
+    <t>33.58719157,-97.91291624</t>
   </si>
 </sst>
 </file>
@@ -556,10 +721,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z6"/>
+  <dimension ref="A1:Z25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -858,6 +1023,449 @@
         <v>49</v>
       </c>
     </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" t="s">
+        <v>45</v>
+      </c>
+      <c r="I7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" t="s">
+        <v>35</v>
+      </c>
+      <c r="H8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" t="s">
+        <v>40</v>
+      </c>
+      <c r="I9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G10" t="s">
+        <v>42</v>
+      </c>
+      <c r="I10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" t="s">
+        <v>48</v>
+      </c>
+      <c r="G11" t="s">
+        <v>48</v>
+      </c>
+      <c r="I11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" t="s">
+        <v>54</v>
+      </c>
+      <c r="G12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" t="s">
+        <v>58</v>
+      </c>
+      <c r="G13" t="s">
+        <v>59</v>
+      </c>
+      <c r="I13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" t="s">
+        <v>63</v>
+      </c>
+      <c r="G14" t="s">
+        <v>64</v>
+      </c>
+      <c r="I14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15" t="s">
+        <v>35</v>
+      </c>
+      <c r="I15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G16" t="s">
+        <v>69</v>
+      </c>
+      <c r="I16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" t="s">
+        <v>72</v>
+      </c>
+      <c r="E17" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" t="s">
+        <v>73</v>
+      </c>
+      <c r="G17" t="s">
+        <v>74</v>
+      </c>
+      <c r="I17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" t="s">
+        <v>76</v>
+      </c>
+      <c r="C18" t="s">
+        <v>77</v>
+      </c>
+      <c r="E18" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18" t="s">
+        <v>78</v>
+      </c>
+      <c r="G18" t="s">
+        <v>79</v>
+      </c>
+      <c r="I18" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" t="s">
+        <v>81</v>
+      </c>
+      <c r="C19" t="s">
+        <v>82</v>
+      </c>
+      <c r="E19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F19" t="s">
+        <v>83</v>
+      </c>
+      <c r="G19" t="s">
+        <v>84</v>
+      </c>
+      <c r="I19" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" t="s">
+        <v>86</v>
+      </c>
+      <c r="C20" t="s">
+        <v>87</v>
+      </c>
+      <c r="E20" t="s">
+        <v>26</v>
+      </c>
+      <c r="F20" t="s">
+        <v>88</v>
+      </c>
+      <c r="G20" t="s">
+        <v>89</v>
+      </c>
+      <c r="I20" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" t="s">
+        <v>91</v>
+      </c>
+      <c r="C21" t="s">
+        <v>87</v>
+      </c>
+      <c r="E21" t="s">
+        <v>26</v>
+      </c>
+      <c r="F21" t="s">
+        <v>88</v>
+      </c>
+      <c r="G21" t="s">
+        <v>89</v>
+      </c>
+      <c r="I21" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" t="s">
+        <v>93</v>
+      </c>
+      <c r="C22" t="s">
+        <v>94</v>
+      </c>
+      <c r="E22" t="s">
+        <v>26</v>
+      </c>
+      <c r="F22" t="s">
+        <v>88</v>
+      </c>
+      <c r="G22" t="s">
+        <v>89</v>
+      </c>
+      <c r="I22" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" t="s">
+        <v>96</v>
+      </c>
+      <c r="C23" t="s">
+        <v>97</v>
+      </c>
+      <c r="E23" t="s">
+        <v>26</v>
+      </c>
+      <c r="F23" t="s">
+        <v>88</v>
+      </c>
+      <c r="G23" t="s">
+        <v>89</v>
+      </c>
+      <c r="I23" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C24" t="s">
+        <v>100</v>
+      </c>
+      <c r="E24" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" t="s">
+        <v>88</v>
+      </c>
+      <c r="G24" t="s">
+        <v>101</v>
+      </c>
+      <c r="I24" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" t="s">
+        <v>103</v>
+      </c>
+      <c r="C25" t="s">
+        <v>94</v>
+      </c>
+      <c r="E25" t="s">
+        <v>26</v>
+      </c>
+      <c r="F25" t="s">
+        <v>104</v>
+      </c>
+      <c r="G25" t="s">
+        <v>105</v>
+      </c>
+      <c r="I25" t="s">
+        <v>106</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>